<commit_message>
fix: KeyError in method conductor_instance
KeyError: 'Worksheet CONDUCTOR_operation does not exist.'

modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_definition.xlsx
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_definition.xlsx
+++ b/TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_definition.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\TDD_examples\CASE_2_ENEA_HTS_CICC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731B21E0-384E-4501-A0C4-CBB53B27F39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D036935-FFB2-49A4-A6C7-A73C011DA433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="4215" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
     <sheet name="CONDUCTOR_input" sheetId="10" r:id="rId2"/>
-    <sheet name="CONDUCTOR_opertation" sheetId="11" r:id="rId3"/>
+    <sheet name="CONDUCTOR_operation" sheetId="11" r:id="rId3"/>
     <sheet name="CONDUCTOR_coupling" sheetId="8" r:id="rId4"/>
   </sheets>
   <externalReferences>
@@ -1098,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D1443-3A2D-4AC0-948E-E6BCBD41CD63}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -1509,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1686A283-62DF-44E8-BE94-5827D9E12853}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix: FileNotFoundError in method save_input_files
FileNotFoundError: [Errno 2] No such file or directory: 'C:/Users/daniele.placido/3D Objects/OPENSC2/TDD_examples/CASE_2_ENEA_HTS_CICC\\alpha.xlsx'

modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_definition.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_definition.xlsx
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_definition.xlsx
+++ b/TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\TDD_examples\CASE_2_ENEA_HTS_CICC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D036935-FFB2-49A4-A6C7-A73C011DA433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF480673-F555-4947-B3CF-443085E18A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="4215" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
   <si>
     <t>m</t>
   </si>
@@ -80,30 +80,15 @@
     <t>EXTERNAL_HEAT</t>
   </si>
   <si>
-    <t>bfield.xlsx</t>
-  </si>
-  <si>
     <t>EXTERNAL_ALPHAB</t>
   </si>
   <si>
     <t>EXTERNAL_STRAIN</t>
   </si>
   <si>
-    <t>alphab_dummy.xlsx</t>
-  </si>
-  <si>
-    <t>strain_dummy.xlsx</t>
-  </si>
-  <si>
-    <t>Q_file_dummy.xlsx</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>I_file_dummy.xlsx</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -119,9 +104,6 @@
     <t>EXTERNAL_FLOW</t>
   </si>
   <si>
-    <t>flow_dummy.xlsx</t>
-  </si>
-  <si>
     <t>XJBEG</t>
   </si>
   <si>
@@ -186,9 +168,6 @@
   </si>
   <si>
     <t>EXTERNAL_GRID</t>
-  </si>
-  <si>
-    <t>spatial_discretization.xlsx</t>
   </si>
   <si>
     <t>custom file name, extension can be xlsx, dat, csv or tsv. Possibility to define a single file with the spatial discretizations for all the conducrors or a file for each conductor (in the last case use different names for the files). No need to have the same extension!</t>
@@ -392,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -407,10 +386,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -826,17 +801,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
@@ -844,10 +819,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8">
         <f>SUM(E2:AE2)</f>
         <v>1</v>
       </c>
@@ -857,234 +832,234 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="9">
+      <c r="D2" s="17"/>
+      <c r="E2" s="8">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="str">
+      <c r="A3" s="10" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="11" t="str">
+      <c r="B3" s="10" t="str">
         <f>[1]TRANSIENT!B$2</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="11" t="str">
+      <c r="C3" s="10" t="str">
         <f>[1]TRANSIENT!C$2</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="11" t="str">
+      <c r="D3" s="10" t="str">
         <f>[1]TRANSIENT!D$2</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="9" t="str">
+      <c r="E3" s="8" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="4" t="s">
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="4" t="s">
+      <c r="E15" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1116,386 +1091,386 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="str">
+      <c r="A1" s="15" t="str">
         <f>CONDUCTOR_files!A$1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="17">
+      <c r="B1" s="16">
         <f>SUM(E2:AE2)</f>
         <v>1</v>
       </c>
-      <c r="E1" s="17">
+      <c r="E1" s="16">
         <f>CONDUCTOR_files!E$1</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="str">
+      <c r="A3" s="15" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="15" t="str">
         <f>CONDUCTOR_files!B$3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="16" t="str">
+      <c r="C3" s="15" t="str">
         <f>CONDUCTOR_files!C$3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="D3" s="15" t="str">
         <f>CONDUCTOR_files!D$3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="17" t="str">
+      <c r="E3" s="16" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>71</v>
+      <c r="A4" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>72</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="E4" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>59</v>
+      <c r="A5" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>60</v>
+        <v>16</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="E5" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>61</v>
+      <c r="A6" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="E6" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>64</v>
+      <c r="A7" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>65</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>75</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>76</v>
+      <c r="A10" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>38</v>
+      <c r="A17" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>37</v>
+        <v>17</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>46</v>
+      <c r="A18" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="10" t="str">
+        <v>18</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="9" t="str">
         <f>E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>52</v>
+      <c r="A19" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>55</v>
+      <c r="A20" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>57</v>
+        <v>16</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>56</v>
+      <c r="A21" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>58</v>
+        <v>16</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>45</v>
+      <c r="A22" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>75</v>
+      <c r="C23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1509,7 +1484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1686A283-62DF-44E8-BE94-5827D9E12853}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1543,143 +1518,143 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="str">
+      <c r="A3" s="22" t="str">
         <f>CONDUCTOR_files!A3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="23" t="str">
+      <c r="B3" s="22" t="str">
         <f>CONDUCTOR_files!B3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="23" t="str">
+      <c r="C3" s="22" t="str">
         <f>CONDUCTOR_files!C3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="23" t="str">
+      <c r="D3" s="22" t="str">
         <f>CONDUCTOR_files!D3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="23" t="str">
+      <c r="E3" s="22" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="E7" s="24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="E8" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="E9" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="25">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="270" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="26">
+      <c r="E10" s="25">
         <v>1</v>
       </c>
     </row>
@@ -1703,13 +1678,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="str">
+      <c r="B1" s="15" t="str">
         <f>CONDUCTOR_files!E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="str">
+      <c r="A2" s="15" t="str">
         <f>B1</f>
         <v>CONDUCTOR_1</v>
       </c>

</xml_diff>